<commit_message>
Created Regression Data with New Design Matrix
</commit_message>
<xml_diff>
--- a/Data for Thesis with New Design Matrix.xlsx
+++ b/Data for Thesis with New Design Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/solbenishay/Desktop/School/2020:21/WInter/Thesis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE99E6A1-DEBD-B34F-A6CE-D88397D44DAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2A2AF6-271C-BD47-835C-856F18F7E136}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1495,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF135"/>
+  <dimension ref="A1:AF133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="Y130" sqref="Y130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1623,27 +1623,27 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="str">
-        <f>A3</f>
+        <f t="shared" ref="A2:F2" si="0">A3</f>
         <v>Airbnb</v>
       </c>
       <c r="B2" s="3" t="str">
-        <f>B3</f>
+        <f t="shared" si="0"/>
         <v>Marriott International</v>
       </c>
       <c r="C2" s="5" t="str">
-        <f>C3</f>
+        <f t="shared" si="0"/>
         <v>MAR</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f>D3</f>
+        <f t="shared" si="0"/>
         <v>NASDAQ</v>
       </c>
       <c r="E2" s="3">
-        <f>E3</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F2" s="3" t="str">
-        <f>F3</f>
+        <f t="shared" si="0"/>
         <v>IXIC</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1738,27 +1738,27 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="str">
-        <f>A5</f>
+        <f t="shared" ref="A4:F4" si="1">A5</f>
         <v>Airbnb</v>
       </c>
       <c r="B4" s="3" t="str">
-        <f>B5</f>
+        <f t="shared" si="1"/>
         <v>Las Vegas Sands</v>
       </c>
       <c r="C4" s="5" t="str">
-        <f>C5</f>
+        <f t="shared" si="1"/>
         <v>LVS</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>D5</f>
+        <f t="shared" si="1"/>
         <v>NYSE</v>
       </c>
       <c r="E4" s="3">
-        <f>E5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F4" s="3" t="str">
-        <f>F5</f>
+        <f t="shared" si="1"/>
         <v>NYA</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1853,27 +1853,27 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="str">
-        <f>A7</f>
+        <f t="shared" ref="A6:F6" si="2">A7</f>
         <v>Bird</v>
       </c>
       <c r="B6" s="3" t="str">
-        <f>B7</f>
+        <f t="shared" si="2"/>
         <v>Giant Manufacturing Co Ltd</v>
       </c>
       <c r="C6" s="5">
-        <f>C7</f>
+        <f t="shared" si="2"/>
         <v>9921</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f>D7</f>
+        <f t="shared" si="2"/>
         <v>TWSE</v>
       </c>
       <c r="E6" s="3">
-        <f>E7</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F6" s="3" t="str">
-        <f>F7</f>
+        <f t="shared" si="2"/>
         <v>TAIEX</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -1968,27 +1968,27 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="str">
-        <f>A9</f>
+        <f t="shared" ref="A8:F8" si="3">A9</f>
         <v>Bird</v>
       </c>
       <c r="B8" s="3" t="str">
-        <f>B9</f>
+        <f t="shared" si="3"/>
         <v>Fox Factory Holding Corp</v>
       </c>
       <c r="C8" s="5" t="str">
-        <f>C9</f>
+        <f t="shared" si="3"/>
         <v>FOXF</v>
       </c>
       <c r="D8" s="3" t="str">
-        <f>D9</f>
+        <f t="shared" si="3"/>
         <v>NASDAQ</v>
       </c>
       <c r="E8" s="3">
-        <f>E9</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F8" s="3" t="str">
-        <f>F9</f>
+        <f t="shared" si="3"/>
         <v>IXIC</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -2083,27 +2083,27 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="str">
-        <f>A11</f>
+        <f t="shared" ref="A10:F10" si="4">A11</f>
         <v>Boatsetter</v>
       </c>
       <c r="B10" s="3" t="str">
-        <f>B11</f>
+        <f t="shared" si="4"/>
         <v>Brunswick Corp</v>
       </c>
       <c r="C10" s="5" t="str">
-        <f>C11</f>
+        <f t="shared" si="4"/>
         <v>BC</v>
       </c>
       <c r="D10" s="3" t="str">
-        <f>D11</f>
+        <f t="shared" si="4"/>
         <v>NYSE</v>
       </c>
       <c r="E10" s="3">
-        <f>E11</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F10" s="3" t="str">
-        <f>F11</f>
+        <f t="shared" si="4"/>
         <v>NYA</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -2198,27 +2198,27 @@
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="str">
-        <f>A13</f>
+        <f t="shared" ref="A12:F12" si="5">A13</f>
         <v>Boatsetter</v>
       </c>
       <c r="B12" s="3" t="str">
-        <f>B13</f>
+        <f t="shared" si="5"/>
         <v>Royal Carribean</v>
       </c>
       <c r="C12" s="5" t="str">
-        <f>C13</f>
+        <f t="shared" si="5"/>
         <v>RCL</v>
       </c>
       <c r="D12" s="3" t="str">
-        <f>D13</f>
+        <f t="shared" si="5"/>
         <v>NYSE</v>
       </c>
       <c r="E12" s="3">
-        <f>E13</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F12" s="3" t="str">
-        <f>F13</f>
+        <f t="shared" si="5"/>
         <v>NYA</v>
       </c>
       <c r="G12" s="4" t="s">
@@ -2313,27 +2313,27 @@
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="str">
-        <f>A15</f>
+        <f t="shared" ref="A14:F14" si="6">A15</f>
         <v>Crowdmed</v>
       </c>
       <c r="B14" s="3" t="str">
-        <f>B15</f>
+        <f t="shared" si="6"/>
         <v>CVS</v>
       </c>
       <c r="C14" s="5" t="str">
-        <f>C15</f>
+        <f t="shared" si="6"/>
         <v>CVS</v>
       </c>
       <c r="D14" s="3" t="str">
-        <f>D15</f>
+        <f t="shared" si="6"/>
         <v>NYSE</v>
       </c>
       <c r="E14" s="3">
-        <f>E15</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F14" s="3" t="str">
-        <f>F15</f>
+        <f t="shared" si="6"/>
         <v>NYA</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -2428,27 +2428,27 @@
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="str">
-        <f>A17</f>
+        <f t="shared" ref="A16:F16" si="7">A17</f>
         <v>Crowdmed</v>
       </c>
       <c r="B16" s="3" t="str">
-        <f>B17</f>
+        <f t="shared" si="7"/>
         <v>Pfizer</v>
       </c>
       <c r="C16" s="5" t="str">
-        <f>C17</f>
+        <f t="shared" si="7"/>
         <v>PFE</v>
       </c>
       <c r="D16" s="3" t="str">
-        <f>D17</f>
+        <f t="shared" si="7"/>
         <v>NYSE</v>
       </c>
       <c r="E16" s="3">
-        <f>E17</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F16" s="3" t="str">
-        <f>F17</f>
+        <f t="shared" si="7"/>
         <v>NYA</v>
       </c>
       <c r="G16" s="4" t="s">
@@ -2543,27 +2543,27 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="str">
-        <f>A19</f>
+        <f t="shared" ref="A18:F18" si="8">A19</f>
         <v>Doordash</v>
       </c>
       <c r="B18" s="3" t="str">
-        <f>B19</f>
+        <f t="shared" si="8"/>
         <v>Dominos</v>
       </c>
       <c r="C18" s="5" t="str">
-        <f>C19</f>
+        <f t="shared" si="8"/>
         <v>DPZ</v>
       </c>
       <c r="D18" s="3" t="str">
-        <f>D19</f>
+        <f t="shared" si="8"/>
         <v>NYSE</v>
       </c>
       <c r="E18" s="3">
-        <f>E19</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F18" s="3" t="str">
-        <f>F19</f>
+        <f t="shared" si="8"/>
         <v>NYA</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -2658,27 +2658,27 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="str">
-        <f>A21</f>
+        <f t="shared" ref="A20:F20" si="9">A21</f>
         <v>Doordash</v>
       </c>
       <c r="B20" s="3" t="str">
-        <f>B21</f>
+        <f t="shared" si="9"/>
         <v>Ingles Markets</v>
       </c>
       <c r="C20" s="5" t="str">
-        <f>C21</f>
+        <f t="shared" si="9"/>
         <v>IMKTA</v>
       </c>
       <c r="D20" s="3" t="str">
-        <f>D21</f>
+        <f t="shared" si="9"/>
         <v>NASDAQ</v>
       </c>
       <c r="E20" s="3">
-        <f>E21</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F20" s="3" t="str">
-        <f>F21</f>
+        <f t="shared" si="9"/>
         <v>IXIC</v>
       </c>
       <c r="G20" s="4" t="s">
@@ -2773,27 +2773,27 @@
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="str">
-        <f>A23</f>
+        <f t="shared" ref="A22:F22" si="10">A23</f>
         <v>Ebay</v>
       </c>
       <c r="B22" s="3" t="str">
-        <f>B23</f>
+        <f t="shared" si="10"/>
         <v>BestBuy</v>
       </c>
       <c r="C22" s="5" t="str">
-        <f>C23</f>
+        <f t="shared" si="10"/>
         <v>BBY</v>
       </c>
       <c r="D22" s="3" t="str">
-        <f>D23</f>
+        <f t="shared" si="10"/>
         <v>NYSE</v>
       </c>
       <c r="E22" s="3">
-        <f>E23</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F22" s="3" t="str">
-        <f>F23</f>
+        <f t="shared" si="10"/>
         <v>NYA</v>
       </c>
       <c r="G22" s="4" t="s">
@@ -2888,27 +2888,27 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="str">
-        <f>A25</f>
+        <f t="shared" ref="A24:F24" si="11">A25</f>
         <v>Ebay</v>
       </c>
       <c r="B24" s="3" t="str">
-        <f>B25</f>
+        <f t="shared" si="11"/>
         <v>Target</v>
       </c>
       <c r="C24" s="5" t="str">
-        <f>C25</f>
+        <f t="shared" si="11"/>
         <v>TGT</v>
       </c>
       <c r="D24" s="3" t="str">
-        <f>D25</f>
+        <f t="shared" si="11"/>
         <v>NYSE</v>
       </c>
       <c r="E24" s="3">
-        <f>E25</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F24" s="3" t="str">
-        <f>F25</f>
+        <f t="shared" si="11"/>
         <v>NYA</v>
       </c>
       <c r="G24" s="4" t="s">
@@ -3003,27 +3003,27 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="str">
-        <f>A27</f>
+        <f t="shared" ref="A26:F26" si="12">A27</f>
         <v>Etsy</v>
       </c>
       <c r="B26" s="3" t="str">
-        <f>B27</f>
+        <f t="shared" si="12"/>
         <v>Nordstrom</v>
       </c>
       <c r="C26" s="5" t="str">
-        <f>C27</f>
+        <f t="shared" si="12"/>
         <v>JWN</v>
       </c>
       <c r="D26" s="3" t="str">
-        <f>D27</f>
+        <f t="shared" si="12"/>
         <v>NYSE</v>
       </c>
       <c r="E26" s="3">
-        <f>E27</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="F26" s="3" t="str">
-        <f>F27</f>
+        <f t="shared" si="12"/>
         <v>NYA</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -3118,27 +3118,27 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="str">
-        <f>A29</f>
+        <f t="shared" ref="A28:F28" si="13">A29</f>
         <v>Etsy</v>
       </c>
       <c r="B28" s="3" t="str">
-        <f>B29</f>
+        <f t="shared" si="13"/>
         <v>Walmart</v>
       </c>
       <c r="C28" s="5" t="str">
-        <f>C29</f>
+        <f t="shared" si="13"/>
         <v>WMT</v>
       </c>
       <c r="D28" s="3" t="str">
-        <f>D29</f>
+        <f t="shared" si="13"/>
         <v>NYSE</v>
       </c>
       <c r="E28" s="3">
-        <f>E29</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F28" s="3" t="str">
-        <f>F29</f>
+        <f t="shared" si="13"/>
         <v>NYA</v>
       </c>
       <c r="G28" s="4" t="s">
@@ -3233,27 +3233,27 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="str">
-        <f>A31</f>
+        <f t="shared" ref="A30:F30" si="14">A31</f>
         <v>Fiverr</v>
       </c>
       <c r="B30" s="3" t="str">
-        <f>B31</f>
+        <f t="shared" si="14"/>
         <v>Wipro</v>
       </c>
       <c r="C30" s="5" t="str">
-        <f>C31</f>
+        <f t="shared" si="14"/>
         <v>WIT</v>
       </c>
       <c r="D30" s="3" t="str">
-        <f>D31</f>
+        <f t="shared" si="14"/>
         <v>NYSE</v>
       </c>
       <c r="E30" s="3">
-        <f>E31</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="F30" s="3" t="str">
-        <f>F31</f>
+        <f t="shared" si="14"/>
         <v>NYA</v>
       </c>
       <c r="G30" s="4" t="s">
@@ -3348,27 +3348,27 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="str">
-        <f>A33</f>
+        <f t="shared" ref="A32:F32" si="15">A33</f>
         <v>Fiverr</v>
       </c>
       <c r="B32" s="3" t="str">
-        <f>B33</f>
+        <f t="shared" si="15"/>
         <v>Tata Consultancy Services</v>
       </c>
       <c r="C32" s="5" t="str">
-        <f>C33</f>
+        <f t="shared" si="15"/>
         <v>TCS</v>
       </c>
       <c r="D32" s="3" t="str">
-        <f>D33</f>
+        <f t="shared" si="15"/>
         <v>NSE</v>
       </c>
       <c r="E32" s="3">
-        <f>E33</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="F32" s="3" t="str">
-        <f>F33</f>
+        <f t="shared" si="15"/>
         <v>NIFTY_50</v>
       </c>
       <c r="G32" s="4" t="s">
@@ -3463,27 +3463,27 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="str">
-        <f>A35</f>
+        <f t="shared" ref="A34:F34" si="16">A35</f>
         <v>Flipkey</v>
       </c>
       <c r="B34" s="3" t="str">
-        <f>B35</f>
+        <f t="shared" si="16"/>
         <v>InterContinental Hotels Group PLC</v>
       </c>
       <c r="C34" s="5" t="str">
-        <f>C35</f>
+        <f t="shared" si="16"/>
         <v>IHG</v>
       </c>
       <c r="D34" s="3" t="str">
-        <f>D35</f>
+        <f t="shared" si="16"/>
         <v>NYSE</v>
       </c>
       <c r="E34" s="3">
-        <f>E35</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="F34" s="3" t="str">
-        <f>F35</f>
+        <f t="shared" si="16"/>
         <v>NYA</v>
       </c>
       <c r="G34" s="4" t="s">
@@ -3578,27 +3578,27 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="str">
-        <f>A37</f>
+        <f t="shared" ref="A36:F36" si="17">A37</f>
         <v>Flipkey</v>
       </c>
       <c r="B36" s="3" t="str">
-        <f>B37</f>
+        <f t="shared" si="17"/>
         <v>MGM</v>
       </c>
       <c r="C36" s="5" t="str">
-        <f>C37</f>
+        <f t="shared" si="17"/>
         <v>MGM</v>
       </c>
       <c r="D36" s="3" t="str">
-        <f>D37</f>
+        <f t="shared" si="17"/>
         <v>NYSE</v>
       </c>
       <c r="E36" s="3">
-        <f>E37</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="F36" s="3" t="str">
-        <f>F37</f>
+        <f t="shared" si="17"/>
         <v>NYA</v>
       </c>
       <c r="G36" s="4" t="s">
@@ -3693,27 +3693,27 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="str">
-        <f>A39</f>
+        <f t="shared" ref="A38:F38" si="18">A39</f>
         <v>Roadie</v>
       </c>
       <c r="B38" s="3" t="str">
-        <f>B39</f>
+        <f t="shared" si="18"/>
         <v>UHaul</v>
       </c>
       <c r="C38" s="5" t="str">
-        <f>C39</f>
+        <f t="shared" si="18"/>
         <v>UHAL</v>
       </c>
       <c r="D38" s="3" t="str">
-        <f>D39</f>
+        <f t="shared" si="18"/>
         <v>NASDAQ</v>
       </c>
       <c r="E38" s="3">
-        <f>E39</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="F38" s="3" t="str">
-        <f>F39</f>
+        <f t="shared" si="18"/>
         <v>IXIC</v>
       </c>
       <c r="G38" s="4" t="s">
@@ -3808,27 +3808,27 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="str">
-        <f>A41</f>
+        <f t="shared" ref="A40:F40" si="19">A41</f>
         <v>Roadie</v>
       </c>
       <c r="B40" s="3" t="str">
-        <f>B41</f>
+        <f t="shared" si="19"/>
         <v>UPS</v>
       </c>
       <c r="C40" s="5" t="str">
-        <f>C41</f>
+        <f t="shared" si="19"/>
         <v>UPS</v>
       </c>
       <c r="D40" s="3" t="str">
-        <f>D41</f>
+        <f t="shared" si="19"/>
         <v>NYSE</v>
       </c>
       <c r="E40" s="3">
-        <f>E41</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F40" s="3" t="str">
-        <f>F41</f>
+        <f t="shared" si="19"/>
         <v>NYA</v>
       </c>
       <c r="G40" s="4" t="s">
@@ -3923,27 +3923,27 @@
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="str">
-        <f>A43</f>
+        <f t="shared" ref="A42:F42" si="20">A43</f>
         <v>Freelancer</v>
       </c>
       <c r="B42" s="3" t="str">
-        <f>B43</f>
+        <f t="shared" si="20"/>
         <v>Cognizant</v>
       </c>
       <c r="C42" s="5" t="str">
-        <f>C43</f>
+        <f t="shared" si="20"/>
         <v>CTSH</v>
       </c>
       <c r="D42" s="3" t="str">
-        <f>D43</f>
+        <f t="shared" si="20"/>
         <v>NASDAQ</v>
       </c>
       <c r="E42" s="3">
-        <f>E43</f>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="F42" s="3" t="str">
-        <f>F43</f>
+        <f t="shared" si="20"/>
         <v>IXIC</v>
       </c>
       <c r="G42" s="4" t="s">
@@ -4038,27 +4038,27 @@
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="str">
-        <f>A45</f>
+        <f t="shared" ref="A44:F44" si="21">A45</f>
         <v>Freelancer</v>
       </c>
       <c r="B44" s="3" t="str">
-        <f>B45</f>
+        <f t="shared" si="21"/>
         <v>Accenture</v>
       </c>
       <c r="C44" s="5" t="str">
-        <f>C45</f>
+        <f t="shared" si="21"/>
         <v>ACN</v>
       </c>
       <c r="D44" s="3" t="str">
-        <f>D45</f>
+        <f t="shared" si="21"/>
         <v>NYSE</v>
       </c>
       <c r="E44" s="3">
-        <f>E45</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="F44" s="3" t="str">
-        <f>F45</f>
+        <f t="shared" si="21"/>
         <v>NYA</v>
       </c>
       <c r="G44" s="4" t="s">
@@ -4153,27 +4153,27 @@
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="str">
-        <f>A47</f>
+        <f t="shared" ref="A46:F46" si="22">A47</f>
         <v>Getaround</v>
       </c>
       <c r="B46" s="3" t="str">
-        <f>B47</f>
+        <f t="shared" si="22"/>
         <v>Ford</v>
       </c>
       <c r="C46" s="5" t="str">
-        <f>C47</f>
+        <f t="shared" si="22"/>
         <v>F</v>
       </c>
       <c r="D46" s="3" t="str">
-        <f>D47</f>
+        <f t="shared" si="22"/>
         <v>NYSE</v>
       </c>
       <c r="E46" s="3">
-        <f>E47</f>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="F46" s="3" t="str">
-        <f>F47</f>
+        <f t="shared" si="22"/>
         <v>NYA</v>
       </c>
       <c r="G46" s="4" t="s">
@@ -4268,27 +4268,27 @@
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="str">
-        <f>A49</f>
+        <f t="shared" ref="A48:F48" si="23">A49</f>
         <v>Getaround</v>
       </c>
       <c r="B48" s="3" t="str">
-        <f>B49</f>
+        <f t="shared" si="23"/>
         <v>Advance Auto Parts</v>
       </c>
       <c r="C48" s="5" t="str">
-        <f>C49</f>
+        <f t="shared" si="23"/>
         <v>AAP</v>
       </c>
       <c r="D48" s="3" t="str">
-        <f>D49</f>
+        <f t="shared" si="23"/>
         <v>NYSE</v>
       </c>
       <c r="E48" s="3">
-        <f>E49</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="F48" s="3" t="str">
-        <f>F49</f>
+        <f t="shared" si="23"/>
         <v>NYA</v>
       </c>
       <c r="G48" s="4" t="s">
@@ -4383,27 +4383,27 @@
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="str">
-        <f>A51</f>
+        <f t="shared" ref="A50:F50" si="24">A51</f>
         <v>Grubhub</v>
       </c>
       <c r="B50" s="3" t="str">
-        <f>B51</f>
+        <f t="shared" si="24"/>
         <v>Yum Brands</v>
       </c>
       <c r="C50" s="5" t="str">
-        <f>C51</f>
+        <f t="shared" si="24"/>
         <v>YUM</v>
       </c>
       <c r="D50" s="3" t="str">
-        <f>D51</f>
+        <f t="shared" si="24"/>
         <v>NYSE</v>
       </c>
       <c r="E50" s="3">
-        <f>E51</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="F50" s="3" t="str">
-        <f>F51</f>
+        <f t="shared" si="24"/>
         <v>NYA</v>
       </c>
       <c r="G50" s="4" t="s">
@@ -4498,27 +4498,27 @@
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="str">
-        <f>A53</f>
+        <f t="shared" ref="A52:F52" si="25">A53</f>
         <v>Grubhub</v>
       </c>
       <c r="B52" s="3" t="str">
-        <f>B53</f>
+        <f t="shared" si="25"/>
         <v>Kroger</v>
       </c>
       <c r="C52" s="5" t="str">
-        <f>C53</f>
+        <f t="shared" si="25"/>
         <v>KR</v>
       </c>
       <c r="D52" s="3" t="str">
-        <f>D53</f>
+        <f t="shared" si="25"/>
         <v>NYSE</v>
       </c>
       <c r="E52" s="3">
-        <f>E53</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="F52" s="3" t="str">
-        <f>F53</f>
+        <f t="shared" si="25"/>
         <v>NYA</v>
       </c>
       <c r="G52" s="4" t="s">
@@ -4613,27 +4613,27 @@
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="str">
-        <f>A55</f>
+        <f t="shared" ref="A54:F54" si="26">A55</f>
         <v>Roadie</v>
       </c>
       <c r="B54" s="3" t="str">
-        <f>B55</f>
+        <f t="shared" si="26"/>
         <v>Fedex</v>
       </c>
       <c r="C54" s="5" t="str">
-        <f>C55</f>
+        <f t="shared" si="26"/>
         <v>FDX</v>
       </c>
       <c r="D54" s="3" t="str">
-        <f>D55</f>
+        <f t="shared" si="26"/>
         <v>NYSE</v>
       </c>
       <c r="E54" s="3">
-        <f>E55</f>
+        <f t="shared" si="26"/>
         <v>1</v>
       </c>
       <c r="F54" s="3" t="str">
-        <f>F55</f>
+        <f t="shared" si="26"/>
         <v>NYA</v>
       </c>
       <c r="G54" s="4" t="s">
@@ -4736,27 +4736,27 @@
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="str">
-        <f>A57</f>
+        <f t="shared" ref="A56:F56" si="27">A57</f>
         <v>Roadie</v>
       </c>
       <c r="B56" s="3" t="str">
-        <f>B57</f>
+        <f t="shared" si="27"/>
         <v>Deutsche Post AG - ADR</v>
       </c>
       <c r="C56" s="5" t="str">
-        <f>C57</f>
+        <f t="shared" si="27"/>
         <v>DPSGY</v>
       </c>
       <c r="D56" s="3" t="str">
-        <f>D57</f>
+        <f t="shared" si="27"/>
         <v>OTCMKTS</v>
       </c>
       <c r="E56" s="3">
-        <f>E57</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="F56" s="3" t="str">
-        <f>F57</f>
+        <f t="shared" si="27"/>
         <v>OTCQX</v>
       </c>
       <c r="G56" s="4" t="s">
@@ -4859,27 +4859,27 @@
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="str">
-        <f>A59</f>
+        <f t="shared" ref="A58:F58" si="28">A59</f>
         <v>Instacart</v>
       </c>
       <c r="B58" s="3" t="str">
-        <f>B59</f>
+        <f t="shared" si="28"/>
         <v>Koninklijke Ahold N.V. ADR</v>
       </c>
       <c r="C58" s="5" t="str">
-        <f>C59</f>
+        <f t="shared" si="28"/>
         <v>ADRNY</v>
       </c>
       <c r="D58" s="3" t="str">
-        <f>D59</f>
+        <f t="shared" si="28"/>
         <v>OTCMKTS</v>
       </c>
       <c r="E58" s="3">
-        <f>E59</f>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="F58" s="3" t="str">
-        <f>F59</f>
+        <f t="shared" si="28"/>
         <v>OTCQX</v>
       </c>
       <c r="G58" s="4" t="s">
@@ -4974,27 +4974,27 @@
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="str">
-        <f>A61</f>
+        <f t="shared" ref="A60:F60" si="29">A61</f>
         <v>Instacart</v>
       </c>
       <c r="B60" s="3" t="str">
-        <f>B61</f>
+        <f t="shared" si="29"/>
         <v>Costco</v>
       </c>
       <c r="C60" s="5" t="str">
-        <f>C61</f>
+        <f t="shared" si="29"/>
         <v>COST</v>
       </c>
       <c r="D60" s="3" t="str">
-        <f>D61</f>
+        <f t="shared" si="29"/>
         <v>NASDAQ</v>
       </c>
       <c r="E60" s="3">
-        <f>E61</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="F60" s="3" t="str">
-        <f>F61</f>
+        <f t="shared" si="29"/>
         <v>IXIC</v>
       </c>
       <c r="G60" s="4" t="s">
@@ -5089,27 +5089,27 @@
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="str">
-        <f>A63</f>
+        <f t="shared" ref="A62:F62" si="30">A63</f>
         <v>JustPark</v>
       </c>
       <c r="B62" s="3" t="str">
-        <f>B63</f>
+        <f t="shared" si="30"/>
         <v>SPPlus Corp</v>
       </c>
       <c r="C62" s="5" t="str">
-        <f>C63</f>
+        <f t="shared" si="30"/>
         <v>SP</v>
       </c>
       <c r="D62" s="3" t="str">
-        <f>D63</f>
+        <f t="shared" si="30"/>
         <v>NASDAQ</v>
       </c>
       <c r="E62" s="3">
-        <f>E63</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="F62" s="3" t="str">
-        <f>F63</f>
+        <f t="shared" si="30"/>
         <v>IXIC</v>
       </c>
       <c r="G62" s="4" t="s">
@@ -5204,27 +5204,27 @@
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="str">
-        <f>A65</f>
+        <f t="shared" ref="A64:F64" si="31">A65</f>
         <v>JustPark</v>
       </c>
       <c r="B64" s="3" t="str">
-        <f>B65</f>
+        <f t="shared" si="31"/>
         <v>JLL</v>
       </c>
       <c r="C64" s="5" t="str">
-        <f>C65</f>
+        <f t="shared" si="31"/>
         <v>JLL</v>
       </c>
       <c r="D64" s="3" t="str">
-        <f>D65</f>
+        <f t="shared" si="31"/>
         <v>NYSE</v>
       </c>
       <c r="E64" s="3">
-        <f>E65</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="F64" s="3" t="str">
-        <f>F65</f>
+        <f t="shared" si="31"/>
         <v>NYA</v>
       </c>
       <c r="G64" s="4" t="s">
@@ -5319,27 +5319,27 @@
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="str">
-        <f>A67</f>
+        <f t="shared" ref="A66:F66" si="32">A67</f>
         <v>Lending Club</v>
       </c>
       <c r="B66" s="3" t="str">
-        <f>B67</f>
+        <f t="shared" si="32"/>
         <v>U.S. Bancorp</v>
       </c>
       <c r="C66" s="5" t="str">
-        <f>C67</f>
+        <f t="shared" si="32"/>
         <v>USB</v>
       </c>
       <c r="D66" s="3" t="str">
-        <f>D67</f>
+        <f t="shared" si="32"/>
         <v>NYSE</v>
       </c>
       <c r="E66" s="3">
-        <f>E67</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="F66" s="3" t="str">
-        <f>F67</f>
+        <f t="shared" si="32"/>
         <v>NYA</v>
       </c>
       <c r="G66" s="4" t="s">
@@ -5434,27 +5434,27 @@
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="str">
-        <f>A69</f>
+        <f t="shared" ref="A68:F68" si="33">A69</f>
         <v>Lending Club</v>
       </c>
       <c r="B68" s="3" t="str">
-        <f>B69</f>
+        <f t="shared" si="33"/>
         <v>JPMorgan Chase</v>
       </c>
       <c r="C68" s="5" t="str">
-        <f>C69</f>
+        <f t="shared" si="33"/>
         <v>JPM</v>
       </c>
       <c r="D68" s="3" t="str">
-        <f>D69</f>
+        <f t="shared" si="33"/>
         <v>NYSE</v>
       </c>
       <c r="E68" s="3">
-        <f>E69</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="F68" s="3" t="str">
-        <f>F69</f>
+        <f t="shared" si="33"/>
         <v>NYA</v>
       </c>
       <c r="G68" s="4" t="s">
@@ -5549,27 +5549,27 @@
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="str">
-        <f>A71</f>
+        <f t="shared" ref="A70:F70" si="34">A71</f>
         <v>Lime</v>
       </c>
       <c r="B70" s="3" t="str">
-        <f>B71</f>
+        <f t="shared" si="34"/>
         <v>Harley Davidson</v>
       </c>
       <c r="C70" s="5" t="str">
-        <f>C71</f>
+        <f t="shared" si="34"/>
         <v>HOG</v>
       </c>
       <c r="D70" s="3" t="str">
-        <f>D71</f>
+        <f t="shared" si="34"/>
         <v>NYSE</v>
       </c>
       <c r="E70" s="3">
-        <f>E71</f>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="F70" s="3" t="str">
-        <f>F71</f>
+        <f t="shared" si="34"/>
         <v>NYA</v>
       </c>
       <c r="G70" s="4" t="s">
@@ -5664,27 +5664,27 @@
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="str">
-        <f>A73</f>
+        <f t="shared" ref="A72:F72" si="35">A73</f>
         <v>Lime</v>
       </c>
       <c r="B72" s="3" t="str">
-        <f>B73</f>
+        <f t="shared" si="35"/>
         <v>General Motors</v>
       </c>
       <c r="C72" s="5" t="str">
-        <f>C73</f>
+        <f t="shared" si="35"/>
         <v>GM</v>
       </c>
       <c r="D72" s="3" t="str">
-        <f>D73</f>
+        <f t="shared" si="35"/>
         <v>NYSE</v>
       </c>
       <c r="E72" s="3">
-        <f>E73</f>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="F72" s="3" t="str">
-        <f>F73</f>
+        <f t="shared" si="35"/>
         <v>NYA</v>
       </c>
       <c r="G72" s="4" t="s">
@@ -5779,27 +5779,27 @@
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="str">
-        <f>A75</f>
+        <f t="shared" ref="A74:F74" si="36">A75</f>
         <v>Lyft</v>
       </c>
       <c r="B74" s="3" t="str">
-        <f>B75</f>
+        <f t="shared" si="36"/>
         <v>Enterprise</v>
       </c>
       <c r="C74" s="5" t="str">
-        <f>C75</f>
+        <f t="shared" si="36"/>
         <v>EPD</v>
       </c>
       <c r="D74" s="3" t="str">
-        <f>D75</f>
+        <f t="shared" si="36"/>
         <v>NYSE</v>
       </c>
       <c r="E74" s="3">
-        <f>E75</f>
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
       <c r="F74" s="3" t="str">
-        <f>F75</f>
+        <f t="shared" si="36"/>
         <v>NYA</v>
       </c>
       <c r="G74" s="4" t="s">
@@ -5894,27 +5894,27 @@
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="str">
-        <f>A77</f>
+        <f t="shared" ref="A76:F76" si="37">A77</f>
         <v>Lyft</v>
       </c>
       <c r="B76" s="3" t="str">
-        <f>B77</f>
+        <f t="shared" si="37"/>
         <v>Nissan</v>
       </c>
       <c r="C76" s="5" t="str">
-        <f>C77</f>
+        <f t="shared" si="37"/>
         <v>NSANY</v>
       </c>
       <c r="D76" s="3" t="str">
-        <f>D77</f>
+        <f t="shared" si="37"/>
         <v>OTCMKTS</v>
       </c>
       <c r="E76" s="3">
-        <f>E77</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="F76" s="3" t="str">
-        <f>F77</f>
+        <f t="shared" si="37"/>
         <v>OTCQX</v>
       </c>
       <c r="G76" s="4" t="s">
@@ -6009,27 +6009,27 @@
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="str">
-        <f>A79</f>
+        <f t="shared" ref="A78:F78" si="38">A79</f>
         <v>Neighbor</v>
       </c>
       <c r="B78" s="3" t="str">
-        <f>B79</f>
+        <f t="shared" si="38"/>
         <v>Public Storage</v>
       </c>
       <c r="C78" s="5" t="str">
-        <f>C79</f>
+        <f t="shared" si="38"/>
         <v>PSA</v>
       </c>
       <c r="D78" s="3" t="str">
-        <f>D79</f>
+        <f t="shared" si="38"/>
         <v>NYSE</v>
       </c>
       <c r="E78" s="3">
-        <f>E79</f>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="F78" s="3" t="str">
-        <f>F79</f>
+        <f t="shared" si="38"/>
         <v>NYA</v>
       </c>
       <c r="G78" s="4" t="s">
@@ -6124,27 +6124,27 @@
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="str">
-        <f>A81</f>
+        <f t="shared" ref="A80:F80" si="39">A81</f>
         <v>Neighbor</v>
       </c>
       <c r="B80" s="3" t="str">
-        <f>B81</f>
+        <f t="shared" si="39"/>
         <v>Ryder</v>
       </c>
       <c r="C80" s="5" t="str">
-        <f>C81</f>
+        <f t="shared" si="39"/>
         <v>R</v>
       </c>
       <c r="D80" s="3" t="str">
-        <f>D81</f>
+        <f t="shared" si="39"/>
         <v>NYSE</v>
       </c>
       <c r="E80" s="3">
-        <f>E81</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="F80" s="3" t="str">
-        <f>F81</f>
+        <f t="shared" si="39"/>
         <v>NYA</v>
       </c>
       <c r="G80" s="4" t="s">
@@ -6239,27 +6239,27 @@
     </row>
     <row r="82" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="str">
-        <f>A83</f>
+        <f t="shared" ref="A82:F82" si="40">A83</f>
         <v>Poshmark</v>
       </c>
       <c r="B82" s="3" t="str">
-        <f>B83</f>
+        <f t="shared" si="40"/>
         <v>Macys</v>
       </c>
       <c r="C82" s="5" t="str">
-        <f>C83</f>
+        <f t="shared" si="40"/>
         <v>M</v>
       </c>
       <c r="D82" s="3" t="str">
-        <f>D83</f>
+        <f t="shared" si="40"/>
         <v>NYSE</v>
       </c>
       <c r="E82" s="3">
-        <f>E83</f>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="F82" s="3" t="str">
-        <f>F83</f>
+        <f t="shared" si="40"/>
         <v>NYA</v>
       </c>
       <c r="G82" s="4" t="s">
@@ -6354,27 +6354,27 @@
     </row>
     <row r="84" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="str">
-        <f>A85</f>
+        <f t="shared" ref="A84:F84" si="41">A85</f>
         <v>Poshmark</v>
       </c>
       <c r="B84" s="3" t="str">
-        <f>B85</f>
+        <f t="shared" si="41"/>
         <v>H&amp;M</v>
       </c>
       <c r="C84" s="5" t="str">
-        <f>C85</f>
+        <f t="shared" si="41"/>
         <v>HNNMY</v>
       </c>
       <c r="D84" s="3" t="str">
-        <f>D85</f>
+        <f t="shared" si="41"/>
         <v>OTCMKTS</v>
       </c>
       <c r="E84" s="3">
-        <f>E85</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="F84" s="3" t="str">
-        <f>F85</f>
+        <f t="shared" si="41"/>
         <v>OTCQX</v>
       </c>
       <c r="G84" s="4" t="s">
@@ -6469,27 +6469,27 @@
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="str">
-        <f>A87</f>
+        <f t="shared" ref="A86:F86" si="42">A87</f>
         <v>Postmates</v>
       </c>
       <c r="B86" s="3" t="str">
-        <f>B87</f>
+        <f t="shared" si="42"/>
         <v>Papa Johns</v>
       </c>
       <c r="C86" s="5" t="str">
-        <f>C87</f>
+        <f t="shared" si="42"/>
         <v>PZZA</v>
       </c>
       <c r="D86" s="3" t="str">
-        <f>D87</f>
+        <f t="shared" si="42"/>
         <v>NASDAQ</v>
       </c>
       <c r="E86" s="3">
-        <f>E87</f>
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
       <c r="F86" s="3" t="str">
-        <f>F87</f>
+        <f t="shared" si="42"/>
         <v>IXIC</v>
       </c>
       <c r="G86" s="4" t="s">
@@ -6584,27 +6584,27 @@
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="str">
-        <f>A89</f>
+        <f t="shared" ref="A88:F88" si="43">A89</f>
         <v>Postmates</v>
       </c>
       <c r="B88" s="3" t="str">
-        <f>B89</f>
+        <f t="shared" si="43"/>
         <v>Weis Markets</v>
       </c>
       <c r="C88" s="5" t="str">
-        <f>C89</f>
+        <f t="shared" si="43"/>
         <v>WMK</v>
       </c>
       <c r="D88" s="3" t="str">
-        <f>D89</f>
+        <f t="shared" si="43"/>
         <v>NYSE</v>
       </c>
       <c r="E88" s="3">
-        <f>E89</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="F88" s="3" t="str">
-        <f>F89</f>
+        <f t="shared" si="43"/>
         <v>NYA</v>
       </c>
       <c r="G88" s="4" t="s">
@@ -6699,27 +6699,27 @@
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="str">
-        <f>A91</f>
+        <f t="shared" ref="A90:F90" si="44">A91</f>
         <v>Rover</v>
       </c>
       <c r="B90" s="3" t="str">
-        <f>B91</f>
+        <f t="shared" si="44"/>
         <v>PetSmart</v>
       </c>
       <c r="C90" s="5" t="str">
-        <f>C91</f>
+        <f t="shared" si="44"/>
         <v>PETM</v>
       </c>
       <c r="D90" s="3" t="str">
-        <f>D91</f>
+        <f t="shared" si="44"/>
         <v>NASDAQ</v>
       </c>
       <c r="E90" s="3">
-        <f>E91</f>
+        <f t="shared" si="44"/>
         <v>1</v>
       </c>
       <c r="F90" s="3" t="str">
-        <f>F91</f>
+        <f t="shared" si="44"/>
         <v>IXIC</v>
       </c>
       <c r="G90" s="4" t="s">
@@ -6814,27 +6814,27 @@
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="str">
-        <f>A93</f>
+        <f t="shared" ref="A92:F92" si="45">A93</f>
         <v>Rover</v>
       </c>
       <c r="B92" s="3" t="str">
-        <f>B93</f>
+        <f t="shared" si="45"/>
         <v>IDEXX Laboratories</v>
       </c>
       <c r="C92" s="5" t="str">
-        <f>C93</f>
+        <f t="shared" si="45"/>
         <v>IDXX</v>
       </c>
       <c r="D92" s="3" t="str">
-        <f>D93</f>
+        <f t="shared" si="45"/>
         <v>NASDAQ</v>
       </c>
       <c r="E92" s="3">
-        <f>E93</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="F92" s="3" t="str">
-        <f>F93</f>
+        <f t="shared" si="45"/>
         <v>IXIC</v>
       </c>
       <c r="G92" s="4" t="s">
@@ -6929,27 +6929,27 @@
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="str">
-        <f>A95</f>
+        <f t="shared" ref="A94:F94" si="46">A95</f>
         <v>RVshare</v>
       </c>
       <c r="B94" s="3" t="str">
-        <f>B95</f>
+        <f t="shared" si="46"/>
         <v>Winnebago</v>
       </c>
       <c r="C94" s="5" t="str">
-        <f>C95</f>
+        <f t="shared" si="46"/>
         <v>WGO</v>
       </c>
       <c r="D94" s="3" t="str">
-        <f>D95</f>
+        <f t="shared" si="46"/>
         <v>NYSE</v>
       </c>
       <c r="E94" s="3">
-        <f>E95</f>
+        <f t="shared" si="46"/>
         <v>1</v>
       </c>
       <c r="F94" s="3" t="str">
-        <f>F95</f>
+        <f t="shared" si="46"/>
         <v>NYA</v>
       </c>
       <c r="G94" s="4" t="s">
@@ -7044,27 +7044,27 @@
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="str">
-        <f>A97</f>
+        <f t="shared" ref="A96:F96" si="47">A97</f>
         <v>RVshare</v>
       </c>
       <c r="B96" s="3" t="str">
-        <f>B97</f>
+        <f t="shared" si="47"/>
         <v>Newell Brands</v>
       </c>
       <c r="C96" s="5" t="str">
-        <f>C97</f>
+        <f t="shared" si="47"/>
         <v>NWL</v>
       </c>
       <c r="D96" s="3" t="str">
-        <f>D97</f>
+        <f t="shared" si="47"/>
         <v>NASDAQ</v>
       </c>
       <c r="E96" s="3">
-        <f>E97</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F96" s="3" t="str">
-        <f>F97</f>
+        <f t="shared" si="47"/>
         <v>IXIC</v>
       </c>
       <c r="G96" s="4" t="s">
@@ -7159,27 +7159,27 @@
     </row>
     <row r="98" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="str">
-        <f>A99</f>
+        <f t="shared" ref="A98:F98" si="48">A99</f>
         <v>Sideline Swap</v>
       </c>
       <c r="B98" s="3" t="str">
-        <f>B99</f>
+        <f t="shared" si="48"/>
         <v>Dick's Sporting Goods Inc</v>
       </c>
       <c r="C98" s="5" t="str">
-        <f>C99</f>
+        <f t="shared" si="48"/>
         <v>DKS</v>
       </c>
       <c r="D98" s="3" t="str">
-        <f>D99</f>
+        <f t="shared" si="48"/>
         <v>NYSE</v>
       </c>
       <c r="E98" s="3">
-        <f>E99</f>
+        <f t="shared" si="48"/>
         <v>1</v>
       </c>
       <c r="F98" s="3" t="str">
-        <f>F99</f>
+        <f t="shared" si="48"/>
         <v>NYA</v>
       </c>
       <c r="G98" s="4" t="s">
@@ -7274,27 +7274,27 @@
     </row>
     <row r="100" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="str">
-        <f>A101</f>
+        <f t="shared" ref="A100:F100" si="49">A101</f>
         <v>Sideline Swap</v>
       </c>
       <c r="B100" s="3" t="str">
-        <f>B101</f>
+        <f t="shared" si="49"/>
         <v>Nike Inc</v>
       </c>
       <c r="C100" s="5" t="str">
-        <f>C101</f>
+        <f t="shared" si="49"/>
         <v>NKE</v>
       </c>
       <c r="D100" s="3" t="str">
-        <f>D101</f>
+        <f t="shared" si="49"/>
         <v>NYSE</v>
       </c>
       <c r="E100" s="3">
-        <f>E101</f>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="F100" s="3" t="str">
-        <f>F101</f>
+        <f t="shared" si="49"/>
         <v>NYA</v>
       </c>
       <c r="G100" s="4" t="s">
@@ -7389,27 +7389,27 @@
     </row>
     <row r="102" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="str">
-        <f>A103</f>
+        <f t="shared" ref="A102:F102" si="50">A103</f>
         <v>SitterCity</v>
       </c>
       <c r="B102" s="3" t="str">
-        <f>B103</f>
+        <f t="shared" si="50"/>
         <v>Welltower Inc</v>
       </c>
       <c r="C102" s="5" t="str">
-        <f>C103</f>
+        <f t="shared" si="50"/>
         <v>WELL</v>
       </c>
       <c r="D102" s="3" t="str">
-        <f>D103</f>
+        <f t="shared" si="50"/>
         <v>NYSE</v>
       </c>
       <c r="E102" s="3">
-        <f>E103</f>
+        <f t="shared" si="50"/>
         <v>1</v>
       </c>
       <c r="F102" s="3" t="str">
-        <f>F103</f>
+        <f t="shared" si="50"/>
         <v>NYA</v>
       </c>
       <c r="G102" s="4" t="s">
@@ -7504,27 +7504,27 @@
     </row>
     <row r="104" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="str">
-        <f>A105</f>
+        <f t="shared" ref="A104:F104" si="51">A105</f>
         <v>SitterCity</v>
       </c>
       <c r="B104" s="3" t="str">
-        <f>B105</f>
+        <f t="shared" si="51"/>
         <v>Community Health Systems</v>
       </c>
       <c r="C104" s="5" t="str">
-        <f>C105</f>
+        <f t="shared" si="51"/>
         <v>CYH</v>
       </c>
       <c r="D104" s="3" t="str">
-        <f>D105</f>
+        <f t="shared" si="51"/>
         <v>NYSE</v>
       </c>
       <c r="E104" s="3">
-        <f>E105</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="F104" s="3" t="str">
-        <f>F105</f>
+        <f t="shared" si="51"/>
         <v>NYA</v>
       </c>
       <c r="G104" s="4" t="s">
@@ -7619,27 +7619,27 @@
     </row>
     <row r="106" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="str">
-        <f>A107</f>
+        <f t="shared" ref="A106:F106" si="52">A107</f>
         <v>Spinlister</v>
       </c>
       <c r="B106" s="3" t="str">
-        <f>B107</f>
+        <f t="shared" si="52"/>
         <v>ANTA Sports</v>
       </c>
       <c r="C106" s="5" t="str">
-        <f>C107</f>
+        <f t="shared" si="52"/>
         <v>ANPDF</v>
       </c>
       <c r="D106" s="3" t="str">
-        <f>D107</f>
+        <f t="shared" si="52"/>
         <v>OTCMKTS</v>
       </c>
       <c r="E106" s="3">
-        <f>E107</f>
+        <f t="shared" si="52"/>
         <v>1</v>
       </c>
       <c r="F106" s="3" t="str">
-        <f>F107</f>
+        <f t="shared" si="52"/>
         <v>OTCQX</v>
       </c>
       <c r="G106" s="4" t="s">
@@ -7734,27 +7734,27 @@
     </row>
     <row r="108" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="str">
-        <f>A109</f>
+        <f t="shared" ref="A108:F108" si="53">A109</f>
         <v>Spinlister</v>
       </c>
       <c r="B108" s="3" t="str">
-        <f>B109</f>
+        <f t="shared" si="53"/>
         <v>Big 5 Sporting Goods Corp</v>
       </c>
       <c r="C108" s="5" t="str">
-        <f>C109</f>
+        <f t="shared" si="53"/>
         <v>BGFV</v>
       </c>
       <c r="D108" s="3" t="str">
-        <f>D109</f>
+        <f t="shared" si="53"/>
         <v>NASDAQ</v>
       </c>
       <c r="E108" s="3">
-        <f>E109</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="F108" s="3" t="str">
-        <f>F109</f>
+        <f t="shared" si="53"/>
         <v>IXIC</v>
       </c>
       <c r="G108" s="4" t="s">
@@ -7849,27 +7849,27 @@
     </row>
     <row r="110" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="str">
-        <f>A111</f>
+        <f t="shared" ref="A110:F110" si="54">A111</f>
         <v>TaskRabbit</v>
       </c>
       <c r="B110" s="3" t="str">
-        <f>B111</f>
+        <f t="shared" si="54"/>
         <v>Home Depot</v>
       </c>
       <c r="C110" s="5" t="str">
-        <f>C111</f>
+        <f t="shared" si="54"/>
         <v>HD</v>
       </c>
       <c r="D110" s="3" t="str">
-        <f>D111</f>
+        <f t="shared" si="54"/>
         <v>NYSE</v>
       </c>
       <c r="E110" s="3">
-        <f>E111</f>
+        <f t="shared" si="54"/>
         <v>1</v>
       </c>
       <c r="F110" s="3" t="str">
-        <f>F111</f>
+        <f t="shared" si="54"/>
         <v>NYA</v>
       </c>
       <c r="G110" s="4" t="s">
@@ -7964,27 +7964,27 @@
     </row>
     <row r="112" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="str">
-        <f>A113</f>
+        <f t="shared" ref="A112:F112" si="55">A113</f>
         <v>TaskRabbit</v>
       </c>
       <c r="B112" s="3" t="str">
-        <f>B113</f>
+        <f t="shared" si="55"/>
         <v>Bassett</v>
       </c>
       <c r="C112" s="5" t="str">
-        <f>C113</f>
+        <f t="shared" si="55"/>
         <v>BSET</v>
       </c>
       <c r="D112" s="3" t="str">
-        <f>D113</f>
+        <f t="shared" si="55"/>
         <v>NASDAQ</v>
       </c>
       <c r="E112" s="3">
-        <f>E113</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="F112" s="3" t="str">
-        <f>F113</f>
+        <f t="shared" si="55"/>
         <v>IXIC</v>
       </c>
       <c r="G112" s="4" t="s">
@@ -8079,27 +8079,27 @@
     </row>
     <row r="114" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="str">
-        <f>A115</f>
+        <f t="shared" ref="A114:F114" si="56">A115</f>
         <v>Turo</v>
       </c>
       <c r="B114" s="3" t="str">
-        <f>B115</f>
+        <f t="shared" si="56"/>
         <v>Hertz</v>
       </c>
       <c r="C114" s="5" t="str">
-        <f>C115</f>
+        <f t="shared" si="56"/>
         <v>HTZGQ</v>
       </c>
       <c r="D114" s="3" t="str">
-        <f>D115</f>
+        <f t="shared" si="56"/>
         <v>OTCMKTS</v>
       </c>
       <c r="E114" s="3">
-        <f>E115</f>
+        <f t="shared" si="56"/>
         <v>1</v>
       </c>
       <c r="F114" s="3" t="str">
-        <f>F115</f>
+        <f t="shared" si="56"/>
         <v>OTCQX</v>
       </c>
       <c r="G114" s="4" t="s">
@@ -8194,27 +8194,27 @@
     </row>
     <row r="116" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="str">
-        <f>A117</f>
+        <f t="shared" ref="A116:F116" si="57">A117</f>
         <v>Turo</v>
       </c>
       <c r="B116" s="3" t="str">
-        <f>B117</f>
+        <f t="shared" si="57"/>
         <v>Honda</v>
       </c>
       <c r="C116" s="5" t="str">
-        <f>C117</f>
+        <f t="shared" si="57"/>
         <v>HMC</v>
       </c>
       <c r="D116" s="3" t="str">
-        <f>D117</f>
+        <f t="shared" si="57"/>
         <v>NYSE</v>
       </c>
       <c r="E116" s="3">
-        <f>E117</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="F116" s="3" t="str">
-        <f>F117</f>
+        <f t="shared" si="57"/>
         <v>NYA</v>
       </c>
       <c r="G116" s="4" t="s">
@@ -8309,27 +8309,27 @@
     </row>
     <row r="118" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="str">
-        <f>A119</f>
+        <f t="shared" ref="A118:F118" si="58">A119</f>
         <v>Uber</v>
       </c>
       <c r="B118" s="3" t="str">
-        <f>B119</f>
+        <f t="shared" si="58"/>
         <v>Avis Budget Group</v>
       </c>
       <c r="C118" s="5" t="str">
-        <f>C119</f>
+        <f t="shared" si="58"/>
         <v>CAR</v>
       </c>
       <c r="D118" s="3" t="str">
-        <f>D119</f>
+        <f t="shared" si="58"/>
         <v>NASDAQ</v>
       </c>
       <c r="E118" s="3">
-        <f>E119</f>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="F118" s="3" t="str">
-        <f>F119</f>
+        <f t="shared" si="58"/>
         <v>IXIC</v>
       </c>
       <c r="G118" s="4" t="s">
@@ -8424,27 +8424,27 @@
     </row>
     <row r="120" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="str">
-        <f>A121</f>
+        <f t="shared" ref="A120:F120" si="59">A121</f>
         <v>Uber</v>
       </c>
       <c r="B120" s="3" t="str">
-        <f>B121</f>
+        <f t="shared" si="59"/>
         <v>Toyota</v>
       </c>
       <c r="C120" s="5" t="str">
-        <f>C121</f>
+        <f t="shared" si="59"/>
         <v>TM</v>
       </c>
       <c r="D120" s="3" t="str">
-        <f>D121</f>
+        <f t="shared" si="59"/>
         <v>NYSE</v>
       </c>
       <c r="E120" s="3">
-        <f>E121</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="F120" s="3" t="str">
-        <f>F121</f>
+        <f t="shared" si="59"/>
         <v>NYA</v>
       </c>
       <c r="G120" s="4" t="s">
@@ -8539,27 +8539,27 @@
     </row>
     <row r="122" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="str">
-        <f>A123</f>
+        <f t="shared" ref="A122:F122" si="60">A123</f>
         <v>WeWork</v>
       </c>
       <c r="B122" s="3" t="str">
-        <f>B123</f>
+        <f t="shared" si="60"/>
         <v>Simon Property Group</v>
       </c>
       <c r="C122" s="5" t="str">
-        <f>C123</f>
+        <f t="shared" si="60"/>
         <v>SPG</v>
       </c>
       <c r="D122" s="3" t="str">
-        <f>D123</f>
+        <f t="shared" si="60"/>
         <v>NYSE</v>
       </c>
       <c r="E122" s="3">
-        <f>E123</f>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="F122" s="3" t="str">
-        <f>F123</f>
+        <f t="shared" si="60"/>
         <v>NYA</v>
       </c>
       <c r="G122" s="4" t="s">
@@ -8654,27 +8654,27 @@
     </row>
     <row r="124" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="str">
-        <f>A125</f>
+        <f t="shared" ref="A124:F124" si="61">A125</f>
         <v>WeWork</v>
       </c>
       <c r="B124" s="3" t="str">
-        <f>B125</f>
+        <f t="shared" si="61"/>
         <v>Avalon Bay Communites</v>
       </c>
       <c r="C124" s="5" t="str">
-        <f>C125</f>
+        <f t="shared" si="61"/>
         <v>AVB</v>
       </c>
       <c r="D124" s="3" t="str">
-        <f>D125</f>
+        <f t="shared" si="61"/>
         <v>NYSE</v>
       </c>
       <c r="E124" s="3">
-        <f>E125</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="F124" s="3" t="str">
-        <f>F125</f>
+        <f t="shared" si="61"/>
         <v>NYA</v>
       </c>
       <c r="G124" s="4" t="s">
@@ -8769,27 +8769,27 @@
     </row>
     <row r="126" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="str">
-        <f>A127</f>
+        <f t="shared" ref="A126:F126" si="62">A127</f>
         <v>Facebook</v>
       </c>
       <c r="B126" s="3" t="str">
-        <f>B127</f>
+        <f t="shared" si="62"/>
         <v>New York Times</v>
       </c>
       <c r="C126" s="5" t="str">
-        <f>C127</f>
+        <f t="shared" si="62"/>
         <v>NYT</v>
       </c>
       <c r="D126" s="3" t="str">
-        <f>D127</f>
+        <f t="shared" si="62"/>
         <v>NYSE</v>
       </c>
       <c r="E126" s="3">
-        <f>E127</f>
+        <f t="shared" si="62"/>
         <v>1</v>
       </c>
       <c r="F126" s="3" t="str">
-        <f>F127</f>
+        <f t="shared" si="62"/>
         <v>NYA</v>
       </c>
       <c r="G126" s="4" t="s">
@@ -8884,27 +8884,27 @@
     </row>
     <row r="128" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="str">
-        <f>A129</f>
+        <f t="shared" ref="A128:F128" si="63">A129</f>
         <v>Facebook</v>
       </c>
       <c r="B128" s="3" t="str">
-        <f>B129</f>
+        <f t="shared" si="63"/>
         <v>Disney</v>
       </c>
       <c r="C128" s="5" t="str">
-        <f>C129</f>
+        <f t="shared" si="63"/>
         <v>DIS</v>
       </c>
       <c r="D128" s="3" t="str">
-        <f>D129</f>
+        <f t="shared" si="63"/>
         <v>NYSE</v>
       </c>
       <c r="E128" s="3">
-        <f>E129</f>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="F128" s="3" t="str">
-        <f>F129</f>
+        <f t="shared" si="63"/>
         <v>NYA</v>
       </c>
       <c r="G128" s="4" t="s">
@@ -8999,27 +8999,27 @@
     </row>
     <row r="130" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="str">
-        <f>A131</f>
+        <f t="shared" ref="A130:F130" si="64">A131</f>
         <v>Twitter</v>
       </c>
       <c r="B130" s="3" t="str">
-        <f>B131</f>
+        <f t="shared" si="64"/>
         <v>Viacom</v>
       </c>
       <c r="C130" s="5" t="str">
-        <f>C131</f>
+        <f t="shared" si="64"/>
         <v>VIAC</v>
       </c>
       <c r="D130" s="3" t="str">
-        <f>D131</f>
+        <f t="shared" si="64"/>
         <v>NASDAQ</v>
       </c>
       <c r="E130" s="3">
-        <f>E131</f>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="F130" s="3" t="str">
-        <f>F131</f>
+        <f t="shared" si="64"/>
         <v>IXIC</v>
       </c>
       <c r="G130" s="4" t="s">
@@ -9114,27 +9114,27 @@
     </row>
     <row r="132" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="str">
-        <f>A133</f>
+        <f t="shared" ref="A132:F132" si="65">A133</f>
         <v>Twitter</v>
       </c>
       <c r="B132" s="3" t="str">
-        <f>B133</f>
+        <f t="shared" si="65"/>
         <v>Thomson Reuters Corp</v>
       </c>
       <c r="C132" s="5" t="str">
-        <f>C133</f>
+        <f t="shared" si="65"/>
         <v>TRI</v>
       </c>
       <c r="D132" s="3" t="str">
-        <f>D133</f>
+        <f t="shared" si="65"/>
         <v>NYSE</v>
       </c>
       <c r="E132" s="3">
-        <f>E133</f>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="F132" s="3" t="str">
-        <f>F133</f>
+        <f t="shared" si="65"/>
         <v>NYA</v>
       </c>
       <c r="G132" s="4" t="s">
@@ -9225,58 +9225,6 @@
       </c>
       <c r="V133" s="1">
         <v>39172</v>
-      </c>
-    </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="M134" s="1">
-        <f>M135</f>
-        <v>0</v>
-      </c>
-      <c r="N134" s="1">
-        <f>N135</f>
-        <v>0</v>
-      </c>
-      <c r="Q134" s="1">
-        <f>Q135</f>
-        <v>0</v>
-      </c>
-      <c r="R134" s="1">
-        <f>R135</f>
-        <v>0</v>
-      </c>
-      <c r="U134" s="1">
-        <f>U135</f>
-        <v>0</v>
-      </c>
-      <c r="V134" s="1">
-        <f>V135</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="M135" s="1">
-        <f>M136</f>
-        <v>0</v>
-      </c>
-      <c r="N135" s="1">
-        <f>N136</f>
-        <v>0</v>
-      </c>
-      <c r="Q135" s="1">
-        <f>Q136</f>
-        <v>0</v>
-      </c>
-      <c r="R135" s="1">
-        <f>R136</f>
-        <v>0</v>
-      </c>
-      <c r="U135" s="1">
-        <f>U136</f>
-        <v>0</v>
-      </c>
-      <c r="V135" s="1">
-        <f>V136</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>